<commit_message>
Reorganise and remove unnecessary files
</commit_message>
<xml_diff>
--- a/01-Research-and-Upskilling/01. Skills Matrix.xlsx
+++ b/01-Research-and-Upskilling/01. Skills Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://autuni-my.sharepoint.com/personal/cgr2690_autuni_ac_nz/Documents/Data/COMP702/Part 1/01-Research-and-Upskilling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="8_{66137141-ADF9-4ECB-AD81-B353D293DF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BC2CF64-DCAF-4352-8EBE-572064644266}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="8_{66137141-ADF9-4ECB-AD81-B353D293DF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD256EF3-E5CA-408E-AA99-2233AC324174}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8AC84B8D-F3D1-41F7-AF19-AD754350EDD7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Skills Matrix</t>
   </si>
@@ -123,7 +123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +147,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +191,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -345,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -407,6 +419,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -419,17 +437,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -586,20 +610,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F80FE532-CB7F-4D29-8231-2499368A1400}" name="Table1" displayName="Table1" ref="A2:K11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" dataCellStyle="Normal">
-  <autoFilter ref="A2:K11" xr:uid="{F80FE532-CB7F-4D29-8231-2499368A1400}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{AAA39393-FD11-4530-95ED-8825AFF24109}" name="Team Members" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{16EBF4D5-0D8A-42E8-8B51-C0B503883D1C}" name="Linux Installation and Configuration" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{9FA02024-20D0-4997-A510-1F3591B74069}" name="Linux as Router Configuration" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{4D63CE57-B503-48AC-8208-BCEBEB694EE7}" name="BASH Scripting" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{96CC8CC3-9E64-4CA0-9F99-EA7E360F1308}" name="Subnetting IPv4" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{E78A595E-7791-46E4-95E9-A04C4035D904}" name="Subnetting IPv6" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{4A288C9E-5F03-49D2-B548-CED020C1A257}" name="Understanding of Networking Protocols (TCP/UDP)" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{A974F890-0BEA-4FE1-BA5B-A452D4D6BA1E}" name="iPerf Usage" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{8CE2597D-3DBF-4432-AEF4-2B6FDE67158B}" name="D-ITG Usage" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{1D7BFCD6-3157-48AD-8733-020C8F6204D2}" name="Basic Network Performance Metrics (Throughput, Delay, Jitter, Packet Loss)" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{29BB43B9-68A9-48BB-9EF0-AE5CD9F608B2}" name="Basic Data Analysis Skills" dataDxfId="0" dataCellStyle="Normal"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F80FE532-CB7F-4D29-8231-2499368A1400}" name="Table1" displayName="Table1" ref="A2:L11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" dataCellStyle="Normal">
+  <autoFilter ref="A2:L11" xr:uid="{F80FE532-CB7F-4D29-8231-2499368A1400}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{AAA39393-FD11-4530-95ED-8825AFF24109}" name="Team Members" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{16EBF4D5-0D8A-42E8-8B51-C0B503883D1C}" name="Linux Installation and Configuration" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{9FA02024-20D0-4997-A510-1F3591B74069}" name="Linux as Router Configuration" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{4D63CE57-B503-48AC-8208-BCEBEB694EE7}" name="BASH Scripting" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{96CC8CC3-9E64-4CA0-9F99-EA7E360F1308}" name="Subnetting IPv4" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{E78A595E-7791-46E4-95E9-A04C4035D904}" name="Subnetting IPv6" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{4A288C9E-5F03-49D2-B548-CED020C1A257}" name="Understanding of Networking Protocols (TCP/UDP)" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{A974F890-0BEA-4FE1-BA5B-A452D4D6BA1E}" name="iPerf Usage" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{8CE2597D-3DBF-4432-AEF4-2B6FDE67158B}" name="D-ITG Usage" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{1D7BFCD6-3157-48AD-8733-020C8F6204D2}" name="Basic Network Performance Metrics (Throughput, Delay, Jitter, Packet Loss)" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{29BB43B9-68A9-48BB-9EF0-AE5CD9F608B2}" name="Basic Data Analysis Skills" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{FFDFC51C-8610-45C4-9F2E-D3AEB082934B}" name="Total" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -925,13 +950,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
@@ -946,22 +971,22 @@
     <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="26.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
-    <row r="2" spans="1:11" ht="45">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -995,8 +1020,11 @@
       <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
@@ -1030,8 +1058,12 @@
       <c r="K3" s="6">
         <v>0</v>
       </c>
+      <c r="L3" s="27">
+        <f>SUM(Table1[[#This Row],[Linux Installation and Configuration]:[Basic Data Analysis Skills]])</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
@@ -1065,8 +1097,12 @@
       <c r="K4" s="6">
         <v>1</v>
       </c>
+      <c r="L4" s="27">
+        <f>SUM(Table1[[#This Row],[Linux Installation and Configuration]:[Basic Data Analysis Skills]])</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
@@ -1100,8 +1136,12 @@
       <c r="K5" s="6">
         <v>1</v>
       </c>
+      <c r="L5" s="27">
+        <f>SUM(Table1[[#This Row],[Linux Installation and Configuration]:[Basic Data Analysis Skills]])</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -1135,43 +1175,51 @@
       <c r="K6" s="6">
         <v>0</v>
       </c>
+      <c r="L6" s="27">
+        <f>SUM(Table1[[#This Row],[Linux Installation and Configuration]:[Basic Data Analysis Skills]])</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="22">
         <v>2</v>
       </c>
-      <c r="C7" s="26">
-        <v>0</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26">
-        <v>1</v>
-      </c>
-      <c r="F7" s="26">
-        <v>0</v>
-      </c>
-      <c r="G7" s="26">
-        <v>1</v>
-      </c>
-      <c r="H7" s="26">
-        <v>0</v>
-      </c>
-      <c r="I7" s="26">
-        <v>0</v>
-      </c>
-      <c r="J7" s="26">
-        <v>0</v>
-      </c>
-      <c r="K7" s="26">
-        <v>1</v>
+      <c r="C7" s="22">
+        <v>0</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0</v>
+      </c>
+      <c r="G7" s="22">
+        <v>1</v>
+      </c>
+      <c r="H7" s="22">
+        <v>0</v>
+      </c>
+      <c r="I7" s="22">
+        <v>0</v>
+      </c>
+      <c r="J7" s="22">
+        <v>0</v>
+      </c>
+      <c r="K7" s="22">
+        <v>1</v>
+      </c>
+      <c r="L7" s="27">
+        <f>SUM(Table1[[#This Row],[Linux Installation and Configuration]:[Basic Data Analysis Skills]])</f>
+        <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
@@ -1205,8 +1253,12 @@
       <c r="K8" s="6">
         <v>1</v>
       </c>
+      <c r="L8" s="27">
+        <f>SUM(Table1[[#This Row],[Linux Installation and Configuration]:[Basic Data Analysis Skills]])</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
@@ -1240,8 +1292,12 @@
       <c r="K9" s="14">
         <v>2</v>
       </c>
+      <c r="L9" s="27">
+        <f>SUM(Table1[[#This Row],[Linux Installation and Configuration]:[Basic Data Analysis Skills]])</f>
+        <v>13</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>19</v>
       </c>
@@ -1285,8 +1341,9 @@
         <f>SUM(K3:K9)</f>
         <v>6</v>
       </c>
+      <c r="L10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>20</v>
       </c>
@@ -1330,8 +1387,9 @@
         <f t="shared" si="1"/>
         <v>0.8571428571428571</v>
       </c>
+      <c r="L11" s="28"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1344,22 +1402,22 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1378,7 +1436,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1397,7 +1455,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1409,46 +1467,47 @@
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D13:G13"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2:K11">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="between">
       <formula>0</formula>
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="between">
       <formula>0</formula>
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:K11">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="between">
       <formula>3</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="between">
       <formula>2</formula>
       <formula>2.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="between">
       <formula>1</formula>
       <formula>1.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>